<commit_message>
added some matlab stuff to lab 5 - manipulating the data with different graphing technequies. All very boring stuff
</commit_message>
<xml_diff>
--- a/Lab 5/Vd vs Vs Data pointsxlsx.xlsx
+++ b/Lab 5/Vd vs Vs Data pointsxlsx.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="21600" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="14400" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -294,6 +294,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -301,9 +304,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -586,28 +586,28 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D27" sqref="D27:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="32"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -653,7 +653,7 @@
       <c r="L2" s="6">
         <v>-5.4</v>
       </c>
-      <c r="M2" s="32"/>
+      <c r="M2" s="29"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -667,23 +667,23 @@
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="7"/>
       <c r="H3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="32"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
@@ -1550,9 +1550,6 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1572,9 +1569,6 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1594,9 +1588,6 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1616,9 +1607,6 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1638,9 +1626,6 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1660,9 +1645,6 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1682,9 +1664,6 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1704,9 +1683,6 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -1726,9 +1702,6 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1748,9 +1721,6 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -1770,9 +1740,6 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1792,9 +1759,6 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1814,9 +1778,6 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -1836,9 +1797,6 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1858,9 +1816,6 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -1880,9 +1835,6 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -1902,9 +1854,6 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1924,9 +1873,6 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -1946,9 +1892,6 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -1968,9 +1911,6 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>

</xml_diff>